<commit_message>
2021-08-03 - Retirada de comentários
</commit_message>
<xml_diff>
--- a/contratos_controle/modelos_excel/BM.xlsx
+++ b/contratos_controle/modelos_excel/BM.xlsx
@@ -1658,7 +1658,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1696,7 +1696,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1768,7 +1768,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>

</xml_diff>